<commit_message>
Update Changes and Upgrades from v0.1.xlsx
</commit_message>
<xml_diff>
--- a/v0.5_Steady_State_Mapping/Changes and Upgrades from v0.1.xlsx
+++ b/v0.5_Steady_State_Mapping/Changes and Upgrades from v0.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab0ee2475784414c/Masaüstü/GitHub/Virtual-Engine-Test-Bench/v0.5_Steady_State_Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC10482FA15B70F25BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA3301D9-C8FE-46AC-A965-FED1FE723B31}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_F25DC773A252ABDACC10482FA15B70F25BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0FF808D-22F1-4F9B-897C-DB901531D99F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Action</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Torque is looking more realistic. FMEP model probably needs some verification though</t>
+  </si>
+  <si>
+    <t>Simplistic emissions model</t>
+  </si>
+  <si>
+    <t>For each working condition, emissions for CO2,CO,Nox,THC is estimated</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,9 +484,15 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>

</xml_diff>